<commit_message>
Add net analysis for critical nets in system.
</commit_message>
<xml_diff>
--- a/03-analysis/Power Analysis.xlsx
+++ b/03-analysis/Power Analysis.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Korwinula\Documents\MIDI-Router\03-analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/korwinan/sandbox/MIDI-Router/03-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{24F6FFE6-262D-4DF9-9893-6AEF5737ECEC}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{19B8F602-CF19-4F44-BAC7-312C008E8B10}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{051525F0-2D76-4EDF-9021-A475D103B1CF}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27260" windowHeight="21320" xr2:uid="{051525F0-2D76-4EDF-9021-A475D103B1CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Power" sheetId="1" r:id="rId1"/>
+    <sheet name="Net Loading" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="71">
   <si>
     <t>Supply</t>
   </si>
@@ -68,6 +69,182 @@
   </si>
   <si>
     <t>LED Power</t>
+  </si>
+  <si>
+    <t>Assembly</t>
+  </si>
+  <si>
+    <t>Logic Board</t>
+  </si>
+  <si>
+    <t>MIDI IN1</t>
+  </si>
+  <si>
+    <t>MIDI IN2</t>
+  </si>
+  <si>
+    <t>MIDI IN3</t>
+  </si>
+  <si>
+    <t>MIDI IN4</t>
+  </si>
+  <si>
+    <t>Net-Source</t>
+  </si>
+  <si>
+    <t>Net-Sink</t>
+  </si>
+  <si>
+    <t>MIDI IN1-3V</t>
+  </si>
+  <si>
+    <t>MIDI IN3-3V</t>
+  </si>
+  <si>
+    <t>MIDI IN4-3V</t>
+  </si>
+  <si>
+    <t>MIDI IN2-3V</t>
+  </si>
+  <si>
+    <t>Signal Conditioning Board</t>
+  </si>
+  <si>
+    <t>FPGA IN1</t>
+  </si>
+  <si>
+    <t>FPGA IN2</t>
+  </si>
+  <si>
+    <t>FPGA IN3</t>
+  </si>
+  <si>
+    <t>FPGA IN4</t>
+  </si>
+  <si>
+    <t>FPGA OUT1</t>
+  </si>
+  <si>
+    <t>FPGA OUT2</t>
+  </si>
+  <si>
+    <t>FPGA OUT3</t>
+  </si>
+  <si>
+    <t>FPGA OUT4</t>
+  </si>
+  <si>
+    <t>MIDI OUT1-3V</t>
+  </si>
+  <si>
+    <t>MIDI OUT2-3V</t>
+  </si>
+  <si>
+    <t>MIDI OUT3-3V</t>
+  </si>
+  <si>
+    <t>MIDI OUT4-3V</t>
+  </si>
+  <si>
+    <t>MIDI OUT1</t>
+  </si>
+  <si>
+    <t>MIDI OUT2</t>
+  </si>
+  <si>
+    <t>MIDI OUT3</t>
+  </si>
+  <si>
+    <t>MIDI OUT4</t>
+  </si>
+  <si>
+    <t>REFO clock</t>
+  </si>
+  <si>
+    <t>REFO clk out</t>
+  </si>
+  <si>
+    <t>FPGA clk</t>
+  </si>
+  <si>
+    <t>REFO clk in</t>
+  </si>
+  <si>
+    <t>SPI SCK</t>
+  </si>
+  <si>
+    <t>SPI SS</t>
+  </si>
+  <si>
+    <t>SPI MOSI</t>
+  </si>
+  <si>
+    <t>SPI MISO</t>
+  </si>
+  <si>
+    <t>FPGA SCK</t>
+  </si>
+  <si>
+    <t>FPGA SS</t>
+  </si>
+  <si>
+    <t>FPGA SDI</t>
+  </si>
+  <si>
+    <t>FPGO SDO</t>
+  </si>
+  <si>
+    <t>I2C SCL</t>
+  </si>
+  <si>
+    <t>I2C SDA</t>
+  </si>
+  <si>
+    <t>I2C bus SCL</t>
+  </si>
+  <si>
+    <t>I2C bus SDA</t>
+  </si>
+  <si>
+    <t>MODE LED</t>
+  </si>
+  <si>
+    <t>MODE LED out</t>
+  </si>
+  <si>
+    <t>Load Model</t>
+  </si>
+  <si>
+    <t>resistive</t>
+  </si>
+  <si>
+    <t>capacitive</t>
+  </si>
+  <si>
+    <t>voltage</t>
+  </si>
+  <si>
+    <t>load current
+[mA]</t>
+  </si>
+  <si>
+    <t>Rth
+[kΩ]</t>
+  </si>
+  <si>
+    <t>capacitance
+[pF]</t>
+  </si>
+  <si>
+    <t>frequency
+[MHz]</t>
+  </si>
+  <si>
+    <t>No significant effect</t>
+  </si>
+  <si>
+    <t>Time constant of RC circuit less than 1% of CPU clock.
+No significant effect</t>
   </si>
 </sst>
 </file>
@@ -103,11 +280,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,13 +606,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -451,7 +629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -463,7 +641,7 @@
         <v>3.0600000000000006E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>3.3</v>
       </c>
@@ -475,7 +653,7 @@
         <v>5.3699999999999998E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>1.2</v>
       </c>
@@ -487,7 +665,7 @@
         <v>2.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -502,7 +680,7 @@
         <v>3.3E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -517,7 +695,7 @@
         <v>3.3E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -532,7 +710,7 @@
         <v>3.3E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -551,7 +729,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>3.3</v>
       </c>
@@ -567,7 +745,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -586,7 +764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="B11">
         <v>3.3</v>
       </c>
@@ -602,7 +780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -621,7 +799,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="B13">
         <v>3.3</v>
       </c>
@@ -637,7 +815,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -646,13 +824,874 @@
         <v>0.18207000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="D16">
         <f>D8+D10+D12</f>
         <v>0.15147000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E0FA17-CAA3-434F-B3D1-3C7666269FE8}">
+  <dimension ref="A1:L26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2">
+        <f>5-3.3</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="F2">
+        <f>E2/G2</f>
+        <v>0.255</v>
+      </c>
+      <c r="G2">
+        <f>10*20/(10+20)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="L2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3">
+        <f>5-3.3</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F5" si="0">E3/G3</f>
+        <v>0.255</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G5" si="1">10*20/(10+20)</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="L3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4">
+        <f>5-3.3</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.255</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="L4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5">
+        <f>5-3.3</f>
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.255</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="L5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6">
+        <v>3.3</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J6" s="2">
+        <f>0.5*E6^2*I6/1000000*H6/1000000000000</f>
+        <v>8.5078124999999996E-18</v>
+      </c>
+      <c r="K6" s="2">
+        <f>J6/E6</f>
+        <v>2.5781249999999999E-18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7">
+        <v>3.3</v>
+      </c>
+      <c r="H7">
+        <v>50</v>
+      </c>
+      <c r="I7">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <f t="shared" ref="J7:J25" si="2">0.5*E7^2*I7/1000000*H7/1000000000000</f>
+        <v>8.5078124999999996E-18</v>
+      </c>
+      <c r="K7" s="2">
+        <f t="shared" ref="K7:K25" si="3">J7/E7</f>
+        <v>2.5781249999999999E-18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8">
+        <v>3.3</v>
+      </c>
+      <c r="H8">
+        <v>50</v>
+      </c>
+      <c r="I8">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J8" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5078124999999996E-18</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="3"/>
+        <v>2.5781249999999999E-18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9">
+        <v>3.3</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="I9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J9" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5078124999999996E-18</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" si="3"/>
+        <v>2.5781249999999999E-18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10">
+        <v>3.3</v>
+      </c>
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J10" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5078124999999996E-18</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="3"/>
+        <v>2.5781249999999999E-18</v>
+      </c>
+      <c r="L10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11">
+        <v>3.3</v>
+      </c>
+      <c r="H11">
+        <v>50</v>
+      </c>
+      <c r="I11">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J11" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5078124999999996E-18</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="3"/>
+        <v>2.5781249999999999E-18</v>
+      </c>
+      <c r="L11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12">
+        <v>3.3</v>
+      </c>
+      <c r="H12">
+        <v>50</v>
+      </c>
+      <c r="I12">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J12" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5078124999999996E-18</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="3"/>
+        <v>2.5781249999999999E-18</v>
+      </c>
+      <c r="L12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13">
+        <v>3.3</v>
+      </c>
+      <c r="H13">
+        <v>50</v>
+      </c>
+      <c r="I13">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J13" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5078124999999996E-18</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="3"/>
+        <v>2.5781249999999999E-18</v>
+      </c>
+      <c r="L13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>50</v>
+      </c>
+      <c r="I14">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="2"/>
+        <v>1.953125E-17</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="3"/>
+        <v>3.9062500000000003E-18</v>
+      </c>
+      <c r="L14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>50</v>
+      </c>
+      <c r="I15">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="2"/>
+        <v>1.953125E-17</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="3"/>
+        <v>3.9062500000000003E-18</v>
+      </c>
+      <c r="L15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>50</v>
+      </c>
+      <c r="I16">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="2"/>
+        <v>1.953125E-17</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="3"/>
+        <v>3.9062500000000003E-18</v>
+      </c>
+      <c r="L16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="H17">
+        <v>50</v>
+      </c>
+      <c r="I17">
+        <v>3.125E-2</v>
+      </c>
+      <c r="J17" s="2">
+        <f t="shared" si="2"/>
+        <v>1.953125E-17</v>
+      </c>
+      <c r="K17" s="2">
+        <f t="shared" si="3"/>
+        <v>3.9062500000000003E-18</v>
+      </c>
+      <c r="L17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18">
+        <v>3.3</v>
+      </c>
+      <c r="F18" s="2">
+        <f>K19</f>
+        <v>2.6399999999999999E-15</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19">
+        <v>3.3</v>
+      </c>
+      <c r="H19">
+        <v>50</v>
+      </c>
+      <c r="I19">
+        <v>32</v>
+      </c>
+      <c r="J19" s="2">
+        <f t="shared" si="2"/>
+        <v>8.7119999999999996E-15</v>
+      </c>
+      <c r="K19" s="2">
+        <f t="shared" si="3"/>
+        <v>2.6399999999999999E-15</v>
+      </c>
+      <c r="L19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20">
+        <v>3.3</v>
+      </c>
+      <c r="I20">
+        <v>16</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21">
+        <v>3.3</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22">
+        <v>3.3</v>
+      </c>
+      <c r="I22">
+        <v>16</v>
+      </c>
+      <c r="J22" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23">
+        <v>3.3</v>
+      </c>
+      <c r="I23">
+        <v>16</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24">
+        <v>3.3</v>
+      </c>
+      <c r="I24">
+        <v>0.1</v>
+      </c>
+      <c r="J24" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25">
+        <v>3.3</v>
+      </c>
+      <c r="I25">
+        <v>0.1</v>
+      </c>
+      <c r="J25" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26">
+        <v>3.3</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <f>E26/F26</f>
+        <v>1.65</v>
+      </c>
+      <c r="I26">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="L26" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>